<commit_message>
jwt no login | novo BD
</commit_message>
<xml_diff>
--- a/public/colaborador.xlsx
+++ b/public/colaborador.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t xml:space="preserve">Assistente Administrativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joana Dark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engenheiro Quimico</t>
   </si>
 </sst>
 </file>
@@ -101,9 +107,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -161,8 +168,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -288,10 +299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,7 +347,7 @@
       <c r="B4" s="2" t="n">
         <v>1236</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -361,6 +372,22 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Tentativa de solução de fetch e added BD SQLite para teste.
</commit_message>
<xml_diff>
--- a/public/colaborador.xlsx
+++ b/public/colaborador.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Tecnico de Seguranca</t>
   </si>
   <si>
-    <t xml:space="preserve">Carlos Santos</t>
+    <t xml:space="preserve">Carla Santos</t>
   </si>
   <si>
     <t xml:space="preserve">Ana Pereira</t>
@@ -71,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -111,6 +111,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -168,12 +173,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -302,7 +311,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,10 +393,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>